<commit_message>
switching browsers working fine
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -12,17 +12,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
-  <si>
-    <t>Row Index</t>
-  </si>
-  <si>
-    <t>Product Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Product Detail</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
+    <t>Meridian Round Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹5,939</t>
+  </si>
+  <si>
+    <t>Adele Rectangular Engineered Wood Coffee Table In Classic Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹2,927</t>
+  </si>
+  <si>
+    <t>Awdry Rectangular Engineered Wood Coffee Table In Sonoma Oak Finish</t>
+  </si>
+  <si>
+    <t>₹2,903</t>
+  </si>
+  <si>
     <t>Altura Rectangular Solid Wood Coffee Table In Two Tone Finish</t>
   </si>
   <si>
@@ -59,27 +77,60 @@
     <t>₹15,317</t>
   </si>
   <si>
+    <t>Dyson Abstract Metal Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹7,679</t>
+  </si>
+  <si>
     <t>Ivara Rectangular Solid Wood Coffee Table In Natural Finish</t>
   </si>
   <si>
     <t>₹16,049</t>
   </si>
   <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹9,647</t>
+  </si>
+  <si>
     <t>Zephyr Rectangular Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
     <t>₹14,104</t>
   </si>
   <si>
+    <t>Fring Engineered Wood Side Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,399</t>
+  </si>
+  <si>
     <t>Claire Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
     <t>Epsilon Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
     <t>₹11,384</t>
   </si>
   <si>
+    <t>Dyson Rectangular Metal Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹10,529</t>
+  </si>
+  <si>
+    <t>Gustowe Rectangular Engineered Wood Coffee Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,279</t>
+  </si>
+  <si>
     <t>Striado Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
@@ -89,12 +140,33 @@
     <t>₹15,677</t>
   </si>
   <si>
+    <t>₹8,374</t>
+  </si>
+  <si>
     <t>Sylvie Rectangular Solid Wood Coffee Table In Natural Finish</t>
   </si>
   <si>
     <t>₹11,839</t>
   </si>
   <si>
+    <t>Liam Rectangular Engineered Wood Coffee Table In Dark Wenge Finish</t>
+  </si>
+  <si>
+    <t>₹3,817</t>
+  </si>
+  <si>
+    <t>Florence Oval Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹10,223</t>
+  </si>
+  <si>
+    <t>Reeves Rectangular Engineered Wood Coffee Table In Rustic Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹5,543</t>
+  </si>
+  <si>
     <t>Nitara Oval Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
@@ -104,67 +176,13 @@
     <t>Renesme Rectangular Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
+    <t>Odette Square Solid Wood Coffee Table In Honey Oak Finish</t>
+  </si>
+  <si>
+    <t>₹5,919</t>
+  </si>
+  <si>
     <t>Epsilon Rectangular Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>Anny Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹27,284</t>
-  </si>
-  <si>
-    <t>Robert Rectangular Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹13,999</t>
-  </si>
-  <si>
-    <t>Blane Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹19,499</t>
-  </si>
-  <si>
-    <t>Rigby Round Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹17,273</t>
-  </si>
-  <si>
-    <t>Milan Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹13,498</t>
-  </si>
-  <si>
-    <t>Montreal Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹11,498</t>
-  </si>
-  <si>
-    <t>Leena Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹28,648</t>
-  </si>
-  <si>
-    <t>Faye Rectangular Metal Coffee Table In Stainless Steel Finish</t>
-  </si>
-  <si>
-    <t>Harry Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Laatto Rectangular Solid Wood Coffee Table In Melamine Finish</t>
-  </si>
-  <si>
-    <t>₹22,040</t>
-  </si>
-  <si>
-    <t>Daniel Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹25,762</t>
   </si>
 </sst>
 </file>
@@ -322,7 +340,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -330,10 +348,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -341,10 +359,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -352,10 +370,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
@@ -363,10 +381,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -374,10 +392,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -385,10 +403,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -396,10 +414,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
@@ -407,10 +425,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -418,10 +436,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
@@ -429,10 +447,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -440,10 +458,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -451,10 +469,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23">
@@ -462,10 +480,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24">
@@ -473,10 +491,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25">
@@ -484,10 +502,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -495,10 +513,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27">
@@ -506,10 +524,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -517,10 +535,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
@@ -528,10 +546,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
@@ -539,10 +557,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -550,10 +568,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>